<commit_message>
feat: remove session persistence tests and add smoke test suite
- Deleted session-persistence.spec.ts to streamline testing focus.
- Introduced smoke-test.spec.ts to validate critical user workflows including upload, view, drag, filter, and export functionalities.
- Added statistics-tab.spec.ts to ensure proper display and functionality of the statistics tab.
- Updated dragAndDrop.ts to improve drag-and-drop functionality using manual mouse events.
- Modified FileUploadDialog to change "Upload" to "Import" for consistency.
- Enhanced AppBar to dynamically display employee count with filters applied.
- Updated ExclusionDialog and FilterDrawer to include data-testid attributes for better testability.
- Adjusted GridBox and NineBoxGrid tests to reflect changes in label formatting.
- Removed timestamp display from ChangeTrackerTab while ensuring correct column visibility.
- Updated vitest.config.ts to include test files for better coverage.
</commit_message>
<xml_diff>
--- a/frontend/playwright/fixtures/sample-employees.xlsx
+++ b/frontend/playwright/fixtures/sample-employees.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Employees" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Employees" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>